<commit_message>
added master search testing functionality
</commit_message>
<xml_diff>
--- a/DPWork_2.O_AutomationTesting/testdata/masterSearch_testdata.xlsx
+++ b/DPWork_2.O_AutomationTesting/testdata/masterSearch_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DP_WORK_2.O\DPWork_2.O\DPWork_2.O_AutomationTesting\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3946E8F-5136-4675-A2E7-5BD596CBD288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9688F16E-7A47-4B4B-993C-40906B748D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4632" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalSearch" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B3C912-42A3-4B91-863B-BD7B27D5AF73}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49103B23-8EB4-4A42-A041-1F5C4D724578}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added end to end testcase py file
</commit_message>
<xml_diff>
--- a/DPWork_2.O_AutomationTesting/testdata/masterSearch_testdata.xlsx
+++ b/DPWork_2.O_AutomationTesting/testdata/masterSearch_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DP_WORK_2.O\DPWork_2.O\DPWork_2.O_AutomationTesting\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9688F16E-7A47-4B4B-993C-40906B748D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8CA4F9-A22C-41CE-BF68-07C373540872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalSearch" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>FieldParameters</t>
   </si>
@@ -138,6 +138,84 @@
   </si>
   <si>
     <t>000053341600</t>
+  </si>
+  <si>
+    <t>Sibu Hazra</t>
+  </si>
+  <si>
+    <t>Ashis Pradhan</t>
+  </si>
+  <si>
+    <t>Ashis</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Pradhan</t>
+  </si>
+  <si>
+    <t>Kumuda</t>
+  </si>
+  <si>
+    <t>Chandra</t>
+  </si>
+  <si>
+    <t>Parimal</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>D-75, Housing Board Colony, Balco, Korba</t>
+  </si>
+  <si>
+    <t>09-03-2008</t>
+  </si>
+  <si>
+    <t>495684</t>
+  </si>
+  <si>
+    <t>Chhattisgarh</t>
+  </si>
+  <si>
+    <t>Korba</t>
+  </si>
+  <si>
+    <t>Jyotirmay</t>
+  </si>
+  <si>
+    <t>Jagadish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chandra </t>
+  </si>
+  <si>
+    <t>sahu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baikuntha </t>
+  </si>
+  <si>
+    <t>nath</t>
+  </si>
+  <si>
+    <t>baripada</t>
+  </si>
+  <si>
+    <t>odisha</t>
+  </si>
+  <si>
+    <t>Mayurbhanj</t>
+  </si>
+  <si>
+    <t>23-05-2007</t>
+  </si>
+  <si>
+    <t>757001</t>
+  </si>
+  <si>
+    <t>500168667400</t>
   </si>
 </sst>
 </file>
@@ -487,20 +565,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,19 +592,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +617,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,10 +657,10 @@
         <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>23</v>
@@ -596,11 +675,9 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
@@ -616,10 +693,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>25</v>
@@ -636,10 +713,10 @@
         <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>26</v>
@@ -656,10 +733,10 @@
         <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>31</v>
@@ -676,10 +753,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>25</v>
@@ -696,10 +773,10 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>27</v>
@@ -716,10 +793,10 @@
         <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>31</v>
@@ -736,10 +813,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>28</v>
@@ -756,10 +833,10 @@
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>29</v>
@@ -776,10 +853,10 @@
         <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>30</v>
@@ -796,10 +873,10 @@
         <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>32</v>
@@ -816,10 +893,10 @@
         <v>33</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>33</v>
@@ -836,10 +913,10 @@
         <v>34</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>34</v>
@@ -852,20 +929,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49103B23-8EB4-4A42-A041-1F5C4D724578}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,22 +951,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added many page object files
</commit_message>
<xml_diff>
--- a/DPWork_2.O_AutomationTesting/testdata/masterSearch_testdata.xlsx
+++ b/DPWork_2.O_AutomationTesting/testdata/masterSearch_testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DP_WORK_2.O\DPWork_2.O\DPWork_2.O_AutomationTesting\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8CA4F9-A22C-41CE-BF68-07C373540872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29EF7AF-37F6-4126-85A5-3F74EA63BDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalSearch" sheetId="1" r:id="rId1"/>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B3C912-42A3-4B91-863B-BD7B27D5AF73}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49103B23-8EB4-4A42-A041-1F5C4D724578}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>